<commit_message>
All changes made is for testing purposes only. No abnormalities occured during testing.
</commit_message>
<xml_diff>
--- a/Withdrawal_Tracking/Withdrawal_History_2024-12.xlsx
+++ b/Withdrawal_Tracking/Withdrawal_History_2024-12.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Withdrawal Control Number</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>WS-2412-008</t>
+  </si>
+  <si>
+    <t>WS-2412-009</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
@@ -656,6 +659,24 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>HYPERLINK("C:/Users/admin/git-directories/Data_Management/Inventory_Management/Withdrawals/WS-2412-009_Jane.pdf", "WS-2412-009_Jane.pdf")</f>
+        <v>WS-2412-009_Jane.pdf</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>